<commit_message>
choire: replace file translation to seperate folder
</commit_message>
<xml_diff>
--- a/data/report.xlsx
+++ b/data/report.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
@@ -44,15 +44,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -168,7 +168,7 @@
           </marker>
           <val>
             <numRef>
-              <f>'Sheet'!$B$2:$B$72</f>
+              <f>'Sheet'!$B$2:$B$85</f>
             </numRef>
           </val>
         </ser>
@@ -195,7 +195,7 @@
           </marker>
           <val>
             <numRef>
-              <f>'Sheet'!$C$2:$C$72</f>
+              <f>'Sheet'!$C$2:$C$85</f>
             </numRef>
           </val>
         </ser>
@@ -308,7 +308,7 @@
           </marker>
           <val>
             <numRef>
-              <f>'Sheet'!$F$2:$F$72</f>
+              <f>'Sheet'!$F$2:$F$85</f>
             </numRef>
           </val>
         </ser>
@@ -715,7 +715,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J73"/>
+  <dimension ref="A1:J86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -780,34 +780,34 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>5.905432698928744</v>
+        <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>5.9048</v>
+        <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>2.44</v>
+        <v>1</v>
       </c>
       <c r="E2" t="n">
-        <v>2.42</v>
+        <v>1</v>
       </c>
       <c r="F2" t="n">
-        <v>0.0006326989287437357</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>106</v>
+        <v>255</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>0x6a</t>
+          <t>0xff</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>107</v>
+        <v>255</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>0x6b</t>
+          <t>0xff</t>
         </is>
       </c>
     </row>
@@ -816,34 +816,34 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>7.825767244953119</v>
+        <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>7.833600000000001</v>
+        <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>2.88</v>
+        <v>1</v>
       </c>
       <c r="E3" t="n">
-        <v>2.72</v>
+        <v>1</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.007832755046881523</v>
+        <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>87</v>
+        <v>255</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>0x57</t>
+          <t>0xff</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>95</v>
+        <v>255</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>0x5f</t>
+          <t>0xff</t>
         </is>
       </c>
     </row>
@@ -852,34 +852,34 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>9.894359013636747</v>
+        <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>9.899999999999999</v>
+        <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>3.3</v>
+        <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.005640986363252054</v>
+        <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>78</v>
+        <v>255</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>0x4e</t>
+          <t>0xff</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>84</v>
+        <v>255</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>0x54</t>
+          <t>0xff</t>
         </is>
       </c>
     </row>
@@ -888,34 +888,34 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>12.12016663427038</v>
+        <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>12.075</v>
+        <v>1</v>
       </c>
       <c r="D5" t="n">
-        <v>3.5</v>
+        <v>1</v>
       </c>
       <c r="E5" t="n">
-        <v>3.45</v>
+        <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>0.04516663427038381</v>
+        <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>74</v>
+        <v>255</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>0x4a</t>
+          <t>0xff</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>75</v>
+        <v>255</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>0x4b</t>
+          <t>0xff</t>
         </is>
       </c>
     </row>
@@ -924,34 +924,34 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>14.51263534723371</v>
+        <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>14.4905</v>
+        <v>1</v>
       </c>
       <c r="D6" t="n">
-        <v>3.97</v>
+        <v>1</v>
       </c>
       <c r="E6" t="n">
-        <v>3.65</v>
+        <v>1</v>
       </c>
       <c r="F6" t="n">
-        <v>0.02213534723370536</v>
+        <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>64</v>
+        <v>255</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>0x40</t>
+          <t>0xff</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>71</v>
+        <v>255</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>0x47</t>
+          <t>0xff</t>
         </is>
       </c>
     </row>
@@ -960,34 +960,34 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>17.08172189721936</v>
+        <v>1.0404</v>
       </c>
       <c r="C7" t="n">
-        <v>17.071</v>
+        <v>1.0404</v>
       </c>
       <c r="D7" t="n">
-        <v>4.3</v>
+        <v>1.02</v>
       </c>
       <c r="E7" t="n">
-        <v>3.97</v>
+        <v>1.02</v>
       </c>
       <c r="F7" t="n">
-        <v>0.01072189721935857</v>
+        <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>60</v>
+        <v>250</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>0x3c</t>
+          <t>0xfa</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>64</v>
+        <v>250</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>0x40</t>
+          <t>0xfa</t>
         </is>
       </c>
     </row>
@@ -996,34 +996,34 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>19.83792065179747</v>
+        <v>1.221</v>
       </c>
       <c r="C8" t="n">
-        <v>19.8</v>
+        <v>1.221</v>
       </c>
       <c r="D8" t="n">
-        <v>4.5</v>
+        <v>1.11</v>
       </c>
       <c r="E8" t="n">
-        <v>4.4</v>
+        <v>1.1</v>
       </c>
       <c r="F8" t="n">
-        <v>0.03792065179747084</v>
+        <v>-2.220446049250313e-16</v>
       </c>
       <c r="G8" t="n">
-        <v>58</v>
+        <v>231</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>0x3a</t>
+          <t>0xe7</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>59</v>
+        <v>233</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>0x3b</t>
+          <t>0xe9</t>
         </is>
       </c>
     </row>
@@ -1032,34 +1032,34 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>22.79229100403987</v>
+        <v>1.4042</v>
       </c>
       <c r="C9" t="n">
-        <v>22.79</v>
+        <v>1.4042</v>
       </c>
       <c r="D9" t="n">
-        <v>5.3</v>
+        <v>1.19</v>
       </c>
       <c r="E9" t="n">
-        <v>4.3</v>
+        <v>1.18</v>
       </c>
       <c r="F9" t="n">
-        <v>0.002291004039868483</v>
+        <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>50</v>
+        <v>216</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>0x32</t>
+          <t>0xd8</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>60</v>
+        <v>218</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>0x3c</t>
+          <t>0xda</t>
         </is>
       </c>
     </row>
@@ -1068,34 +1068,34 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>25.956486120681</v>
+        <v>1.6002</v>
       </c>
       <c r="C10" t="n">
-        <v>25.97</v>
+        <v>1.6002</v>
       </c>
       <c r="D10" t="n">
-        <v>5.3</v>
+        <v>1.27</v>
       </c>
       <c r="E10" t="n">
-        <v>4.9</v>
+        <v>1.26</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.01351387931900305</v>
+        <v>-2.220446049250313e-16</v>
       </c>
       <c r="G10" t="n">
-        <v>50</v>
+        <v>202</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>0x32</t>
+          <t>0xca</t>
         </is>
       </c>
       <c r="I10" t="n">
-        <v>54</v>
+        <v>204</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>0x36</t>
+          <t>0xcc</t>
         </is>
       </c>
     </row>
@@ -1104,34 +1104,34 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>29.34278310017972</v>
+        <v>1.7822</v>
       </c>
       <c r="C11" t="n">
-        <v>29.4</v>
+        <v>1.7822</v>
       </c>
       <c r="D11" t="n">
-        <v>6</v>
+        <v>1.34</v>
       </c>
       <c r="E11" t="n">
-        <v>4.9</v>
+        <v>1.33</v>
       </c>
       <c r="F11" t="n">
-        <v>-0.05721689982027911</v>
+        <v>-2.220446049250313e-16</v>
       </c>
       <c r="G11" t="n">
-        <v>44</v>
+        <v>192</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>0x2c</t>
+          <t>0xc0</t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>54</v>
+        <v>194</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>0x36</t>
+          <t>0xc2</t>
         </is>
       </c>
     </row>
@@ -1140,34 +1140,34 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>32.96411460806552</v>
+        <v>1.974</v>
       </c>
       <c r="C12" t="n">
-        <v>32.94</v>
+        <v>1.974</v>
       </c>
       <c r="D12" t="n">
-        <v>6.1</v>
+        <v>1.41</v>
       </c>
       <c r="E12" t="n">
-        <v>5.4</v>
+        <v>1.4</v>
       </c>
       <c r="F12" t="n">
-        <v>0.02411460806552412</v>
+        <v>-2.220446049250313e-16</v>
       </c>
       <c r="G12" t="n">
-        <v>43</v>
+        <v>183</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>0x2b</t>
+          <t>0xb7</t>
         </is>
       </c>
       <c r="I12" t="n">
-        <v>49</v>
+        <v>184</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>0x31</t>
+          <t>0xb8</t>
         </is>
       </c>
     </row>
@@ -1176,34 +1176,34 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>36.8341020601122</v>
+        <v>2.190399999999999</v>
       </c>
       <c r="C13" t="n">
-        <v>36.85</v>
+        <v>2.1904</v>
       </c>
       <c r="D13" t="n">
-        <v>6.7</v>
+        <v>1.48</v>
       </c>
       <c r="E13" t="n">
-        <v>5.5</v>
+        <v>1.48</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.01589793988780031</v>
+        <v>-4.440892098500626e-16</v>
       </c>
       <c r="G13" t="n">
-        <v>39</v>
+        <v>174</v>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>0x27</t>
+          <t>0xae</t>
         </is>
       </c>
       <c r="I13" t="n">
-        <v>48</v>
+        <v>174</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>0x30</t>
+          <t>0xae</t>
         </is>
       </c>
     </row>
@@ -1212,34 +1212,34 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>40.96709042718801</v>
+        <v>2.3562</v>
       </c>
       <c r="C14" t="n">
-        <v>40.96000000000001</v>
+        <v>2.3562</v>
       </c>
       <c r="D14" t="n">
-        <v>6.4</v>
+        <v>1.54</v>
       </c>
       <c r="E14" t="n">
-        <v>6.4</v>
+        <v>1.53</v>
       </c>
       <c r="F14" t="n">
-        <v>0.0070904271880039</v>
+        <v>0</v>
       </c>
       <c r="G14" t="n">
-        <v>41</v>
+        <v>167</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>0x29</t>
+          <t>0xa7</t>
         </is>
       </c>
       <c r="I14" t="n">
-        <v>41</v>
+        <v>168</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>0x29</t>
+          <t>0xa8</t>
         </is>
       </c>
     </row>
@@ -1248,34 +1248,34 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>45.37818473908818</v>
+        <v>2.56</v>
       </c>
       <c r="C15" t="n">
-        <v>45.36</v>
+        <v>2.56</v>
       </c>
       <c r="D15" t="n">
-        <v>7.2</v>
+        <v>1.6</v>
       </c>
       <c r="E15" t="n">
-        <v>6.3</v>
+        <v>1.6</v>
       </c>
       <c r="F15" t="n">
-        <v>0.01818473908817708</v>
+        <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>36</v>
+        <v>160</v>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>0x24</t>
+          <t>0xa0</t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>42</v>
+        <v>160</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>0x2a</t>
+          <t>0xa0</t>
         </is>
       </c>
     </row>
@@ -1284,34 +1284,34 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>50.08328836827464</v>
+        <v>2.755599999999999</v>
       </c>
       <c r="C16" t="n">
-        <v>49.92</v>
+        <v>2.7556</v>
       </c>
       <c r="D16" t="n">
-        <v>7.8</v>
+        <v>1.66</v>
       </c>
       <c r="E16" t="n">
-        <v>6.4</v>
+        <v>1.66</v>
       </c>
       <c r="F16" t="n">
-        <v>0.1632883682746424</v>
+        <v>-4.440892098500626e-16</v>
       </c>
       <c r="G16" t="n">
-        <v>32</v>
+        <v>155</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>0x20</t>
+          <t>0x9b</t>
         </is>
       </c>
       <c r="I16" t="n">
-        <v>41</v>
+        <v>155</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>0x29</t>
+          <t>0x9b</t>
         </is>
       </c>
     </row>
@@ -1320,34 +1320,34 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>55.09914317823166</v>
+        <v>2.9929</v>
       </c>
       <c r="C17" t="n">
-        <v>55.25</v>
+        <v>2.9929</v>
       </c>
       <c r="D17" t="n">
-        <v>8.5</v>
+        <v>1.73</v>
       </c>
       <c r="E17" t="n">
-        <v>6.5</v>
+        <v>1.73</v>
       </c>
       <c r="F17" t="n">
-        <v>-0.1508568217683433</v>
+        <v>-4.440892098500626e-16</v>
       </c>
       <c r="G17" t="n">
-        <v>30</v>
+        <v>149</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>0x1e</t>
+          <t>0x95</t>
         </is>
       </c>
       <c r="I17" t="n">
-        <v>40</v>
+        <v>149</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>0x28</t>
+          <t>0x95</t>
         </is>
       </c>
     </row>
@@ -1356,34 +1356,34 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>60.44337162510493</v>
+        <v>3.186199999999999</v>
       </c>
       <c r="C18" t="n">
-        <v>60.3</v>
+        <v>3.1862</v>
       </c>
       <c r="D18" t="n">
-        <v>9</v>
+        <v>1.79</v>
       </c>
       <c r="E18" t="n">
-        <v>6.7</v>
+        <v>1.78</v>
       </c>
       <c r="F18" t="n">
-        <v>0.1433716251049262</v>
+        <v>-4.440892098500626e-16</v>
       </c>
       <c r="G18" t="n">
-        <v>29</v>
+        <v>144</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>0x1d</t>
+          <t>0x90</t>
         </is>
       </c>
       <c r="I18" t="n">
-        <v>39</v>
+        <v>145</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>0x27</t>
+          <t>0x91</t>
         </is>
       </c>
     </row>
@@ -1392,34 +1392,34 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>66.13452090543369</v>
+        <v>3.3855</v>
       </c>
       <c r="C19" t="n">
-        <v>66.3</v>
+        <v>3.3855</v>
       </c>
       <c r="D19" t="n">
-        <v>8.5</v>
+        <v>1.85</v>
       </c>
       <c r="E19" t="n">
-        <v>7.8</v>
+        <v>1.83</v>
       </c>
       <c r="F19" t="n">
-        <v>-0.165479094566308</v>
+        <v>-4.440892098500626e-16</v>
       </c>
       <c r="G19" t="n">
-        <v>30</v>
+        <v>139</v>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>0x1e</t>
+          <t>0x8b</t>
         </is>
       </c>
       <c r="I19" t="n">
-        <v>32</v>
+        <v>140</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>0x20</t>
+          <t>0x8c</t>
         </is>
       </c>
     </row>
@@ -1428,34 +1428,34 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>72.192109247117</v>
+        <v>3.5721</v>
       </c>
       <c r="C20" t="n">
-        <v>72.2</v>
+        <v>3.5721</v>
       </c>
       <c r="D20" t="n">
-        <v>9.5</v>
+        <v>1.89</v>
       </c>
       <c r="E20" t="n">
-        <v>7.6</v>
+        <v>1.89</v>
       </c>
       <c r="F20" t="n">
-        <v>-0.007890752883000118</v>
+        <v>0</v>
       </c>
       <c r="G20" t="n">
-        <v>27</v>
+        <v>136</v>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>0x1b</t>
+          <t>0x88</t>
         </is>
       </c>
       <c r="I20" t="n">
-        <v>33</v>
+        <v>136</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>0x21</t>
+          <t>0x88</t>
         </is>
       </c>
     </row>
@@ -1464,34 +1464,34 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>78.63667444528909</v>
+        <v>3.8025</v>
       </c>
       <c r="C21" t="n">
-        <v>78.28</v>
+        <v>3.8025</v>
       </c>
       <c r="D21" t="n">
-        <v>10.3</v>
+        <v>1.95</v>
       </c>
       <c r="E21" t="n">
-        <v>7.6</v>
+        <v>1.95</v>
       </c>
       <c r="F21" t="n">
-        <v>0.3566744452890873</v>
+        <v>0</v>
       </c>
       <c r="G21" t="n">
-        <v>25</v>
+        <v>132</v>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>0x19</t>
+          <t>0x84</t>
         </is>
       </c>
       <c r="I21" t="n">
-        <v>33</v>
+        <v>132</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>0x21</t>
+          <t>0x84</t>
         </is>
       </c>
     </row>
@@ -1500,34 +1500,34 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>85.48982474951349</v>
+        <v>4</v>
       </c>
       <c r="C22" t="n">
-        <v>85.5</v>
+        <v>4</v>
       </c>
       <c r="D22" t="n">
-        <v>9.5</v>
+        <v>2</v>
       </c>
       <c r="E22" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="F22" t="n">
-        <v>-0.0101752504865118</v>
+        <v>0</v>
       </c>
       <c r="G22" t="n">
-        <v>27</v>
+        <v>129</v>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>0x1b</t>
+          <t>0x81</t>
         </is>
       </c>
       <c r="I22" t="n">
-        <v>29</v>
+        <v>129</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>0x1d</t>
+          <t>0x81</t>
         </is>
       </c>
     </row>
@@ -1536,34 +1536,34 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>92.77429221367272</v>
+        <v>4.243599999999999</v>
       </c>
       <c r="C23" t="n">
-        <v>92.7</v>
+        <v>4.2436</v>
       </c>
       <c r="D23" t="n">
-        <v>10.3</v>
+        <v>2.06</v>
       </c>
       <c r="E23" t="n">
-        <v>9</v>
+        <v>2.06</v>
       </c>
       <c r="F23" t="n">
-        <v>0.07429221367272021</v>
+        <v>-8.881784197001252e-16</v>
       </c>
       <c r="G23" t="n">
-        <v>25</v>
+        <v>125</v>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>0x19</t>
+          <t>0x7d</t>
         </is>
       </c>
       <c r="I23" t="n">
-        <v>29</v>
+        <v>125</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>0x1d</t>
+          <t>0x7d</t>
         </is>
       </c>
     </row>
@@ -1572,34 +1572,34 @@
         <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>100.5139886251069</v>
+        <v>4.452000000000001</v>
       </c>
       <c r="C24" t="n">
-        <v>100.8</v>
+        <v>4.452000000000001</v>
       </c>
       <c r="D24" t="n">
-        <v>11.2</v>
+        <v>2.12</v>
       </c>
       <c r="E24" t="n">
-        <v>9</v>
+        <v>2.1</v>
       </c>
       <c r="F24" t="n">
-        <v>-0.2860113748930502</v>
+        <v>0</v>
       </c>
       <c r="G24" t="n">
-        <v>23</v>
+        <v>122</v>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>0x17</t>
+          <t>0x7a</t>
         </is>
       </c>
       <c r="I24" t="n">
-        <v>29</v>
+        <v>123</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>0x1d</t>
+          <t>0x7b</t>
         </is>
       </c>
     </row>
@@ -1608,34 +1608,34 @@
         <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>108.7340641349867</v>
+        <v>4.644</v>
       </c>
       <c r="C25" t="n">
-        <v>108</v>
+        <v>4.644</v>
       </c>
       <c r="D25" t="n">
-        <v>12</v>
+        <v>2.16</v>
       </c>
       <c r="E25" t="n">
-        <v>9</v>
+        <v>2.15</v>
       </c>
       <c r="F25" t="n">
-        <v>0.734064134986653</v>
+        <v>0</v>
       </c>
       <c r="G25" t="n">
-        <v>22</v>
+        <v>119</v>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>0x16</t>
+          <t>0x77</t>
         </is>
       </c>
       <c r="I25" t="n">
-        <v>29</v>
+        <v>120</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>0x1d</t>
+          <t>0x78</t>
         </is>
       </c>
     </row>
@@ -1644,34 +1644,34 @@
         <v>25</v>
       </c>
       <c r="B26" t="n">
-        <v>117.4609687175749</v>
+        <v>4.906000000000001</v>
       </c>
       <c r="C26" t="n">
+        <v>4.906000000000001</v>
+      </c>
+      <c r="D26" t="n">
+        <v>2.23</v>
+      </c>
+      <c r="E26" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0</v>
+      </c>
+      <c r="G26" t="n">
+        <v>116</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>0x74</t>
+        </is>
+      </c>
+      <c r="I26" t="n">
         <v>117</v>
       </c>
-      <c r="D26" t="n">
-        <v>13</v>
-      </c>
-      <c r="E26" t="n">
-        <v>9</v>
-      </c>
-      <c r="F26" t="n">
-        <v>0.4609687175748718</v>
-      </c>
-      <c r="G26" t="n">
-        <v>20</v>
-      </c>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t>0x14</t>
-        </is>
-      </c>
-      <c r="I26" t="n">
-        <v>29</v>
-      </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>0x1d</t>
+          <t>0x75</t>
         </is>
       </c>
     </row>
@@ -1680,34 +1680,34 @@
         <v>26</v>
       </c>
       <c r="B27" t="n">
-        <v>126.7225165919684</v>
+        <v>5.107599999999999</v>
       </c>
       <c r="C27" t="n">
-        <v>126.69</v>
+        <v>5.107599999999999</v>
       </c>
       <c r="D27" t="n">
-        <v>12.3</v>
+        <v>2.26</v>
       </c>
       <c r="E27" t="n">
-        <v>10.3</v>
+        <v>2.26</v>
       </c>
       <c r="F27" t="n">
-        <v>0.03251659196834567</v>
+        <v>0</v>
       </c>
       <c r="G27" t="n">
-        <v>21</v>
+        <v>114</v>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>0x15</t>
+          <t>0x72</t>
         </is>
       </c>
       <c r="I27" t="n">
-        <v>25</v>
+        <v>114</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>0x19</t>
+          <t>0x72</t>
         </is>
       </c>
     </row>
@@ -1716,34 +1716,34 @@
         <v>27</v>
       </c>
       <c r="B28" t="n">
-        <v>136.5479537461158</v>
+        <v>5.335999999999999</v>
       </c>
       <c r="C28" t="n">
-        <v>137.76</v>
+        <v>5.335999999999999</v>
       </c>
       <c r="D28" t="n">
-        <v>12.3</v>
+        <v>2.32</v>
       </c>
       <c r="E28" t="n">
-        <v>11.2</v>
+        <v>2.3</v>
       </c>
       <c r="F28" t="n">
-        <v>-1.212046253884211</v>
+        <v>-8.881784197001252e-16</v>
       </c>
       <c r="G28" t="n">
-        <v>21</v>
+        <v>111</v>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>0x15</t>
+          <t>0x6f</t>
         </is>
       </c>
       <c r="I28" t="n">
-        <v>23</v>
+        <v>112</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>0x17</t>
+          <t>0x70</t>
         </is>
       </c>
     </row>
@@ -1752,34 +1752,34 @@
         <v>28</v>
       </c>
       <c r="B29" t="n">
-        <v>146.9680287093987</v>
+        <v>5.664399999999999</v>
       </c>
       <c r="C29" t="n">
-        <v>147.6</v>
+        <v>5.6644</v>
       </c>
       <c r="D29" t="n">
-        <v>12.3</v>
+        <v>2.38</v>
       </c>
       <c r="E29" t="n">
-        <v>12</v>
+        <v>2.38</v>
       </c>
       <c r="F29" t="n">
-        <v>-0.6319712906013422</v>
+        <v>-8.881784197001252e-16</v>
       </c>
       <c r="G29" t="n">
-        <v>21</v>
+        <v>109</v>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>0x15</t>
+          <t>0x6d</t>
         </is>
       </c>
       <c r="I29" t="n">
-        <v>22</v>
+        <v>109</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>0x16</t>
+          <t>0x6d</t>
         </is>
       </c>
     </row>
@@ -1788,34 +1788,34 @@
         <v>29</v>
       </c>
       <c r="B30" t="n">
-        <v>158.0150667268552</v>
+        <v>5.9048</v>
       </c>
       <c r="C30" t="n">
-        <v>156.8</v>
+        <v>5.9048</v>
       </c>
       <c r="D30" t="n">
-        <v>14</v>
+        <v>2.44</v>
       </c>
       <c r="E30" t="n">
-        <v>11.2</v>
+        <v>2.42</v>
       </c>
       <c r="F30" t="n">
-        <v>1.215066726855213</v>
+        <v>0</v>
       </c>
       <c r="G30" t="n">
-        <v>18</v>
+        <v>106</v>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>0x12</t>
+          <t>0x6a</t>
         </is>
       </c>
       <c r="I30" t="n">
-        <v>23</v>
+        <v>107</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>0x17</t>
+          <t>0x6b</t>
         </is>
       </c>
     </row>
@@ -1824,34 +1824,34 @@
         <v>30</v>
       </c>
       <c r="B31" t="n">
-        <v>169.7230474952158</v>
+        <v>6.175000000000001</v>
       </c>
       <c r="C31" t="n">
-        <v>169.95</v>
+        <v>6.175000000000001</v>
       </c>
       <c r="D31" t="n">
-        <v>16.5</v>
+        <v>2.5</v>
       </c>
       <c r="E31" t="n">
-        <v>10.3</v>
+        <v>2.47</v>
       </c>
       <c r="F31" t="n">
-        <v>-0.226952504784208</v>
+        <v>0</v>
       </c>
       <c r="G31" t="n">
-        <v>15</v>
+        <v>104</v>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>0xf</t>
+          <t>0x68</t>
         </is>
       </c>
       <c r="I31" t="n">
-        <v>25</v>
+        <v>105</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>0x19</t>
+          <t>0x69</t>
         </is>
       </c>
     </row>
@@ -1860,34 +1860,34 @@
         <v>31</v>
       </c>
       <c r="B32" t="n">
-        <v>182.1276866283639</v>
+        <v>6.577999999999999</v>
       </c>
       <c r="C32" t="n">
-        <v>182.25</v>
+        <v>6.577999999999999</v>
       </c>
       <c r="D32" t="n">
-        <v>13.5</v>
+        <v>2.6</v>
       </c>
       <c r="E32" t="n">
-        <v>13.5</v>
+        <v>2.53</v>
       </c>
       <c r="F32" t="n">
-        <v>-0.1223133716360962</v>
+        <v>-8.881784197001252e-16</v>
       </c>
       <c r="G32" t="n">
-        <v>19</v>
+        <v>101</v>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>0x13</t>
+          <t>0x65</t>
         </is>
       </c>
       <c r="I32" t="n">
-        <v>19</v>
+        <v>103</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>0x13</t>
+          <t>0x67</t>
         </is>
       </c>
     </row>
@@ -1896,34 +1896,34 @@
         <v>32</v>
       </c>
       <c r="B33" t="n">
-        <v>195.2665210275719</v>
+        <v>6.968000000000001</v>
       </c>
       <c r="C33" t="n">
-        <v>195</v>
+        <v>6.968000000000001</v>
       </c>
       <c r="D33" t="n">
-        <v>15</v>
+        <v>2.68</v>
       </c>
       <c r="E33" t="n">
-        <v>13</v>
+        <v>2.6</v>
       </c>
       <c r="F33" t="n">
-        <v>0.266521027571855</v>
+        <v>0</v>
       </c>
       <c r="G33" t="n">
-        <v>17</v>
+        <v>99</v>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>0x11</t>
+          <t>0x63</t>
         </is>
       </c>
       <c r="I33" t="n">
-        <v>20</v>
+        <v>101</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>0x14</t>
+          <t>0x65</t>
         </is>
       </c>
     </row>
@@ -1932,34 +1932,34 @@
         <v>33</v>
       </c>
       <c r="B34" t="n">
-        <v>209.1789983400154</v>
+        <v>7.2092</v>
       </c>
       <c r="C34" t="n">
-        <v>209</v>
+        <v>7.2092</v>
       </c>
       <c r="D34" t="n">
-        <v>19</v>
+        <v>2.69</v>
       </c>
       <c r="E34" t="n">
-        <v>11</v>
+        <v>2.68</v>
       </c>
       <c r="F34" t="n">
-        <v>0.1789983400154256</v>
+        <v>0</v>
       </c>
       <c r="G34" t="n">
-        <v>14</v>
+        <v>98</v>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>0xe</t>
+          <t>0x62</t>
         </is>
       </c>
       <c r="I34" t="n">
-        <v>24</v>
+        <v>99</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>0x18</t>
+          <t>0x63</t>
         </is>
       </c>
     </row>
@@ -1968,34 +1968,34 @@
         <v>34</v>
       </c>
       <c r="B35" t="n">
-        <v>223.9065706975303</v>
+        <v>7.316999999999999</v>
       </c>
       <c r="C35" t="n">
-        <v>224</v>
+        <v>7.317</v>
       </c>
       <c r="D35" t="n">
-        <v>20</v>
+        <v>2.71</v>
       </c>
       <c r="E35" t="n">
-        <v>11.2</v>
+        <v>2.7</v>
       </c>
       <c r="F35" t="n">
-        <v>-0.09342930246967285</v>
+        <v>-8.881784197001252e-16</v>
       </c>
       <c r="G35" t="n">
-        <v>13</v>
+        <v>96</v>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>0xd</t>
+          <t>0x60</t>
         </is>
       </c>
       <c r="I35" t="n">
-        <v>23</v>
+        <v>97</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>0x17</t>
+          <t>0x61</t>
         </is>
       </c>
     </row>
@@ -2004,34 +2004,34 @@
         <v>35</v>
       </c>
       <c r="B36" t="n">
-        <v>239.4927929364793</v>
+        <v>7.452800000000001</v>
       </c>
       <c r="C36" t="n">
-        <v>240</v>
+        <v>7.452800000000001</v>
       </c>
       <c r="D36" t="n">
-        <v>20</v>
+        <v>2.74</v>
       </c>
       <c r="E36" t="n">
-        <v>12</v>
+        <v>2.72</v>
       </c>
       <c r="F36" t="n">
-        <v>-0.507207063520724</v>
+        <v>0</v>
       </c>
       <c r="G36" t="n">
-        <v>13</v>
+        <v>94</v>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>0xd</t>
+          <t>0x5e</t>
         </is>
       </c>
       <c r="I36" t="n">
-        <v>22</v>
+        <v>95</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>0x16</t>
+          <t>0x5f</t>
         </is>
       </c>
     </row>
@@ -2040,34 +2040,34 @@
         <v>36</v>
       </c>
       <c r="B37" t="n">
-        <v>255.9834255088701</v>
+        <v>7.617599999999998</v>
       </c>
       <c r="C37" t="n">
-        <v>256.5</v>
+        <v>7.617599999999999</v>
       </c>
       <c r="D37" t="n">
-        <v>19</v>
+        <v>2.76</v>
       </c>
       <c r="E37" t="n">
-        <v>13.5</v>
+        <v>2.76</v>
       </c>
       <c r="F37" t="n">
-        <v>-0.5165744911299157</v>
+        <v>-8.881784197001252e-16</v>
       </c>
       <c r="G37" t="n">
-        <v>14</v>
+        <v>93</v>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>0xe</t>
+          <t>0x5d</t>
         </is>
       </c>
       <c r="I37" t="n">
-        <v>19</v>
+        <v>93</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>0x13</t>
+          <t>0x5d</t>
         </is>
       </c>
     </row>
@@ -2076,34 +2076,34 @@
         <v>37</v>
       </c>
       <c r="B38" t="n">
-        <v>273.426542304574</v>
+        <v>7.756199999999999</v>
       </c>
       <c r="C38" t="n">
-        <v>272.25</v>
+        <v>7.7562</v>
       </c>
       <c r="D38" t="n">
-        <v>16.5</v>
+        <v>2.79</v>
       </c>
       <c r="E38" t="n">
-        <v>16.5</v>
+        <v>2.78</v>
       </c>
       <c r="F38" t="n">
-        <v>1.176542304573957</v>
+        <v>-8.881784197001252e-16</v>
       </c>
       <c r="G38" t="n">
-        <v>15</v>
+        <v>91</v>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>0xf</t>
+          <t>0x5b</t>
         </is>
       </c>
       <c r="I38" t="n">
-        <v>15</v>
+        <v>92</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>0xf</t>
+          <t>0x5c</t>
         </is>
       </c>
     </row>
@@ -2112,34 +2112,34 @@
         <v>38</v>
       </c>
       <c r="B39" t="n">
-        <v>291.8726436146658</v>
+        <v>7.867799999999999</v>
       </c>
       <c r="C39" t="n">
-        <v>295.2</v>
+        <v>7.8678</v>
       </c>
       <c r="D39" t="n">
-        <v>24</v>
+        <v>2.82</v>
       </c>
       <c r="E39" t="n">
-        <v>12.3</v>
+        <v>2.79</v>
       </c>
       <c r="F39" t="n">
-        <v>-3.327356385334269</v>
+        <v>-8.881784197001252e-16</v>
       </c>
       <c r="G39" t="n">
-        <v>11</v>
+        <v>89</v>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>0xb</t>
+          <t>0x59</t>
         </is>
       </c>
       <c r="I39" t="n">
-        <v>21</v>
+        <v>91</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>0x15</t>
+          <t>0x5b</t>
         </is>
       </c>
     </row>
@@ -2148,34 +2148,34 @@
         <v>39</v>
       </c>
       <c r="B40" t="n">
-        <v>311.3747744764933</v>
+        <v>8.121599999999999</v>
       </c>
       <c r="C40" t="n">
-        <v>312</v>
+        <v>8.121599999999999</v>
       </c>
       <c r="D40" t="n">
-        <v>24</v>
+        <v>2.88</v>
       </c>
       <c r="E40" t="n">
-        <v>13</v>
+        <v>2.82</v>
       </c>
       <c r="F40" t="n">
-        <v>-0.6252255235066855</v>
+        <v>0</v>
       </c>
       <c r="G40" t="n">
-        <v>11</v>
+        <v>87</v>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>0xb</t>
+          <t>0x57</t>
         </is>
       </c>
       <c r="I40" t="n">
-        <v>20</v>
+        <v>89</v>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>0x14</t>
+          <t>0x59</t>
         </is>
       </c>
     </row>
@@ -2184,34 +2184,34 @@
         <v>40</v>
       </c>
       <c r="B41" t="n">
-        <v>331.988648652218</v>
+        <v>8.264999999999999</v>
       </c>
       <c r="C41" t="n">
-        <v>330</v>
+        <v>8.265000000000001</v>
       </c>
       <c r="D41" t="n">
-        <v>22</v>
+        <v>2.9</v>
       </c>
       <c r="E41" t="n">
-        <v>15</v>
+        <v>2.85</v>
       </c>
       <c r="F41" t="n">
-        <v>1.988648652217989</v>
+        <v>-1.77635683940025e-15</v>
       </c>
       <c r="G41" t="n">
-        <v>12</v>
+        <v>86</v>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>0xc</t>
+          <t>0x56</t>
         </is>
       </c>
       <c r="I41" t="n">
-        <v>17</v>
+        <v>88</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>0x11</t>
+          <t>0x58</t>
         </is>
       </c>
     </row>
@@ -2220,34 +2220,34 @@
         <v>41</v>
       </c>
       <c r="B42" t="n">
-        <v>353.7727785041502</v>
+        <v>8.555</v>
       </c>
       <c r="C42" t="n">
-        <v>351</v>
+        <v>8.555</v>
       </c>
       <c r="D42" t="n">
-        <v>26</v>
+        <v>2.95</v>
       </c>
       <c r="E42" t="n">
-        <v>13.5</v>
+        <v>2.9</v>
       </c>
       <c r="F42" t="n">
-        <v>2.772778504150153</v>
+        <v>0</v>
       </c>
       <c r="G42" t="n">
-        <v>9</v>
+        <v>85</v>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>0x9</t>
+          <t>0x55</t>
         </is>
       </c>
       <c r="I42" t="n">
-        <v>19</v>
+        <v>86</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>0x13</t>
+          <t>0x56</t>
         </is>
       </c>
     </row>
@@ -2256,34 +2256,34 @@
         <v>42</v>
       </c>
       <c r="B43" t="n">
-        <v>376.7886110423601</v>
+        <v>8.850000000000001</v>
       </c>
       <c r="C43" t="n">
-        <v>375</v>
+        <v>8.850000000000001</v>
       </c>
       <c r="D43" t="n">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="E43" t="n">
-        <v>15</v>
+        <v>2.95</v>
       </c>
       <c r="F43" t="n">
-        <v>1.788611042360117</v>
+        <v>0</v>
       </c>
       <c r="G43" t="n">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>0xa</t>
+          <t>0x54</t>
         </is>
       </c>
       <c r="I43" t="n">
-        <v>17</v>
+        <v>85</v>
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>0x11</t>
+          <t>0x55</t>
         </is>
       </c>
     </row>
@@ -2292,34 +2292,34 @@
         <v>43</v>
       </c>
       <c r="B44" t="n">
-        <v>401.1006704327158</v>
+        <v>9.149999999999999</v>
       </c>
       <c r="C44" t="n">
-        <v>400</v>
+        <v>9.149999999999999</v>
       </c>
       <c r="D44" t="n">
-        <v>20</v>
+        <v>3.05</v>
       </c>
       <c r="E44" t="n">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="F44" t="n">
-        <v>1.100670432715845</v>
+        <v>0</v>
       </c>
       <c r="G44" t="n">
-        <v>13</v>
+        <v>83</v>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>0xd</t>
+          <t>0x53</t>
         </is>
       </c>
       <c r="I44" t="n">
-        <v>13</v>
+        <v>84</v>
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>0xd</t>
+          <t>0x54</t>
         </is>
       </c>
     </row>
@@ -2328,34 +2328,34 @@
         <v>44</v>
       </c>
       <c r="B45" t="n">
-        <v>426.7767072667916</v>
+        <v>9.455</v>
       </c>
       <c r="C45" t="n">
-        <v>429</v>
+        <v>9.455</v>
       </c>
       <c r="D45" t="n">
-        <v>26</v>
+        <v>3.1</v>
       </c>
       <c r="E45" t="n">
-        <v>16.5</v>
+        <v>3.05</v>
       </c>
       <c r="F45" t="n">
-        <v>-2.223292733208382</v>
+        <v>0</v>
       </c>
       <c r="G45" t="n">
-        <v>9</v>
+        <v>82</v>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>0x9</t>
+          <t>0x52</t>
         </is>
       </c>
       <c r="I45" t="n">
-        <v>15</v>
+        <v>83</v>
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>0xf</t>
+          <t>0x53</t>
         </is>
       </c>
     </row>
@@ -2364,34 +2364,34 @@
         <v>45</v>
       </c>
       <c r="B46" t="n">
-        <v>453.8878549089321</v>
+        <v>9.765000000000001</v>
       </c>
       <c r="C46" t="n">
-        <v>456</v>
+        <v>9.765000000000001</v>
       </c>
       <c r="D46" t="n">
-        <v>24</v>
+        <v>3.15</v>
       </c>
       <c r="E46" t="n">
-        <v>19</v>
+        <v>3.1</v>
       </c>
       <c r="F46" t="n">
-        <v>-2.11214509106793</v>
+        <v>0</v>
       </c>
       <c r="G46" t="n">
-        <v>11</v>
+        <v>81</v>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>0xb</t>
+          <t>0x51</t>
         </is>
       </c>
       <c r="I46" t="n">
-        <v>14</v>
+        <v>82</v>
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>0xe</t>
+          <t>0x52</t>
         </is>
       </c>
     </row>
@@ -2400,34 +2400,34 @@
         <v>46</v>
       </c>
       <c r="B47" t="n">
-        <v>482.508793250303</v>
+        <v>10.08</v>
       </c>
       <c r="C47" t="n">
-        <v>484</v>
+        <v>10.08</v>
       </c>
       <c r="D47" t="n">
-        <v>22</v>
+        <v>3.2</v>
       </c>
       <c r="E47" t="n">
-        <v>22</v>
+        <v>3.15</v>
       </c>
       <c r="F47" t="n">
-        <v>-1.491206749696971</v>
+        <v>0</v>
       </c>
       <c r="G47" t="n">
-        <v>12</v>
+        <v>80</v>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>0xc</t>
+          <t>0x50</t>
         </is>
       </c>
       <c r="I47" t="n">
-        <v>12</v>
+        <v>81</v>
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>0xc</t>
+          <t>0x51</t>
         </is>
       </c>
     </row>
@@ -2436,34 +2436,34 @@
         <v>47</v>
       </c>
       <c r="B48" t="n">
-        <v>512.7179202148737</v>
+        <v>10.4</v>
       </c>
       <c r="C48" t="n">
-        <v>520</v>
+        <v>10.4</v>
       </c>
       <c r="D48" t="n">
-        <v>26</v>
+        <v>3.25</v>
       </c>
       <c r="E48" t="n">
-        <v>20</v>
+        <v>3.2</v>
       </c>
       <c r="F48" t="n">
-        <v>-7.282079785126257</v>
+        <v>0</v>
       </c>
       <c r="G48" t="n">
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>0x9</t>
+          <t>0x4f</t>
         </is>
       </c>
       <c r="I48" t="n">
-        <v>13</v>
+        <v>80</v>
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>0xd</t>
+          <t>0x50</t>
         </is>
       </c>
     </row>
@@ -2472,34 +2472,34 @@
         <v>48</v>
       </c>
       <c r="B49" t="n">
-        <v>544.5975313781767</v>
+        <v>10.5625</v>
       </c>
       <c r="C49" t="n">
-        <v>550</v>
+        <v>10.5625</v>
       </c>
       <c r="D49" t="n">
-        <v>25</v>
+        <v>3.25</v>
       </c>
       <c r="E49" t="n">
-        <v>22</v>
+        <v>3.25</v>
       </c>
       <c r="F49" t="n">
-        <v>-5.402468621823346</v>
+        <v>-1.77635683940025e-15</v>
       </c>
       <c r="G49" t="n">
-        <v>10</v>
+        <v>79</v>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>0xa</t>
+          <t>0x4f</t>
         </is>
       </c>
       <c r="I49" t="n">
-        <v>12</v>
+        <v>79</v>
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>0xc</t>
+          <t>0x4f</t>
         </is>
       </c>
     </row>
@@ -2508,34 +2508,34 @@
         <v>49</v>
       </c>
       <c r="B50" t="n">
-        <v>578.2340080762309</v>
+        <v>10.89</v>
       </c>
       <c r="C50" t="n">
-        <v>576</v>
+        <v>10.89</v>
       </c>
       <c r="D50" t="n">
-        <v>24</v>
+        <v>3.3</v>
       </c>
       <c r="E50" t="n">
-        <v>24</v>
+        <v>3.3</v>
       </c>
       <c r="F50" t="n">
-        <v>2.234008076230907</v>
+        <v>-1.77635683940025e-15</v>
       </c>
       <c r="G50" t="n">
-        <v>11</v>
+        <v>78</v>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>0xb</t>
+          <t>0x4e</t>
         </is>
       </c>
       <c r="I50" t="n">
-        <v>11</v>
+        <v>78</v>
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>0xb</t>
+          <t>0x4e</t>
         </is>
       </c>
     </row>
@@ -2544,34 +2544,34 @@
         <v>50</v>
       </c>
       <c r="B51" t="n">
-        <v>613.7180143993696</v>
+        <v>11.2225</v>
       </c>
       <c r="C51" t="n">
-        <v>616</v>
+        <v>11.2225</v>
       </c>
       <c r="D51" t="n">
-        <v>28</v>
+        <v>3.35</v>
       </c>
       <c r="E51" t="n">
-        <v>22</v>
+        <v>3.35</v>
       </c>
       <c r="F51" t="n">
-        <v>-2.281985600630378</v>
+        <v>0</v>
       </c>
       <c r="G51" t="n">
-        <v>8</v>
+        <v>77</v>
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>0x8</t>
+          <t>0x4d</t>
         </is>
       </c>
       <c r="I51" t="n">
-        <v>12</v>
+        <v>77</v>
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>0xc</t>
+          <t>0x4d</t>
         </is>
       </c>
     </row>
@@ -2580,34 +2580,34 @@
         <v>51</v>
       </c>
       <c r="B52" t="n">
-        <v>651.1447034837931</v>
+        <v>11.39</v>
       </c>
       <c r="C52" t="n">
-        <v>650</v>
+        <v>11.39</v>
       </c>
       <c r="D52" t="n">
-        <v>26</v>
+        <v>3.4</v>
       </c>
       <c r="E52" t="n">
-        <v>25</v>
+        <v>3.35</v>
       </c>
       <c r="F52" t="n">
-        <v>1.144703483793137</v>
+        <v>0</v>
       </c>
       <c r="G52" t="n">
-        <v>9</v>
+        <v>76</v>
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>0x9</t>
+          <t>0x4c</t>
         </is>
       </c>
       <c r="I52" t="n">
-        <v>10</v>
+        <v>77</v>
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>0xa</t>
+          <t>0x4d</t>
         </is>
       </c>
     </row>
@@ -2616,34 +2616,34 @@
         <v>52</v>
       </c>
       <c r="B53" t="n">
-        <v>690.6139335326607</v>
+        <v>11.73</v>
       </c>
       <c r="C53" t="n">
-        <v>700</v>
+        <v>11.73</v>
       </c>
       <c r="D53" t="n">
-        <v>28</v>
+        <v>3.45</v>
       </c>
       <c r="E53" t="n">
-        <v>25</v>
+        <v>3.4</v>
       </c>
       <c r="F53" t="n">
-        <v>-9.386066467339333</v>
+        <v>-1.77635683940025e-15</v>
       </c>
       <c r="G53" t="n">
-        <v>8</v>
+        <v>75</v>
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>0x8</t>
+          <t>0x4b</t>
         </is>
       </c>
       <c r="I53" t="n">
-        <v>10</v>
+        <v>76</v>
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>0xa</t>
+          <t>0x4c</t>
         </is>
       </c>
     </row>
@@ -2652,34 +2652,34 @@
         <v>53</v>
       </c>
       <c r="B54" t="n">
-        <v>732.2304940182611</v>
+        <v>12.075</v>
       </c>
       <c r="C54" t="n">
-        <v>728</v>
+        <v>12.075</v>
       </c>
       <c r="D54" t="n">
-        <v>28</v>
+        <v>3.5</v>
       </c>
       <c r="E54" t="n">
-        <v>26</v>
+        <v>3.45</v>
       </c>
       <c r="F54" t="n">
-        <v>4.230494018261084</v>
+        <v>0</v>
       </c>
       <c r="G54" t="n">
-        <v>8</v>
+        <v>74</v>
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>0x8</t>
+          <t>0x4a</t>
         </is>
       </c>
       <c r="I54" t="n">
-        <v>9</v>
+        <v>75</v>
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>0x9</t>
+          <t>0x4b</t>
         </is>
       </c>
     </row>
@@ -2688,34 +2688,34 @@
         <v>54</v>
       </c>
       <c r="B55" t="n">
-        <v>776.1043425375707</v>
+        <v>12.25</v>
       </c>
       <c r="C55" t="n">
-        <v>775.5</v>
+        <v>12.25</v>
       </c>
       <c r="D55" t="n">
-        <v>47</v>
+        <v>3.5</v>
       </c>
       <c r="E55" t="n">
-        <v>16.5</v>
+        <v>3.5</v>
       </c>
       <c r="F55" t="n">
-        <v>0.6043425375706875</v>
+        <v>0</v>
       </c>
       <c r="G55" t="n">
-        <v>5</v>
+        <v>74</v>
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>0x5</t>
+          <t>0x4a</t>
         </is>
       </c>
       <c r="I55" t="n">
-        <v>15</v>
+        <v>74</v>
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>0xf</t>
+          <t>0x4a</t>
         </is>
       </c>
     </row>
@@ -2724,34 +2724,34 @@
         <v>55</v>
       </c>
       <c r="B56" t="n">
-        <v>822.3508528150861</v>
+        <v>12.6025</v>
       </c>
       <c r="C56" t="n">
-        <v>832</v>
+        <v>12.6025</v>
       </c>
       <c r="D56" t="n">
-        <v>32</v>
+        <v>3.55</v>
       </c>
       <c r="E56" t="n">
-        <v>26</v>
+        <v>3.55</v>
       </c>
       <c r="F56" t="n">
-        <v>-9.649147184913886</v>
+        <v>0</v>
       </c>
       <c r="G56" t="n">
-        <v>7</v>
+        <v>73</v>
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>0x7</t>
+          <t>0x49</t>
         </is>
       </c>
       <c r="I56" t="n">
-        <v>9</v>
+        <v>73</v>
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>0x9</t>
+          <t>0x49</t>
         </is>
       </c>
     </row>
@@ -2760,34 +2760,34 @@
         <v>56</v>
       </c>
       <c r="B57" t="n">
-        <v>871.0910743694748</v>
+        <v>12.96</v>
       </c>
       <c r="C57" t="n">
-        <v>893</v>
+        <v>12.96</v>
       </c>
       <c r="D57" t="n">
-        <v>47</v>
+        <v>3.6</v>
       </c>
       <c r="E57" t="n">
-        <v>19</v>
+        <v>3.6</v>
       </c>
       <c r="F57" t="n">
-        <v>-21.90892563052523</v>
+        <v>0</v>
       </c>
       <c r="G57" t="n">
-        <v>5</v>
+        <v>72</v>
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>0x5</t>
+          <t>0x48</t>
         </is>
       </c>
       <c r="I57" t="n">
-        <v>14</v>
+        <v>72</v>
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t>0xe</t>
+          <t>0x48</t>
         </is>
       </c>
     </row>
@@ -2796,34 +2796,34 @@
         <v>57</v>
       </c>
       <c r="B58" t="n">
-        <v>922.452004384182</v>
+        <v>13.14</v>
       </c>
       <c r="C58" t="n">
-        <v>912</v>
+        <v>13.14</v>
       </c>
       <c r="D58" t="n">
-        <v>38</v>
+        <v>3.65</v>
       </c>
       <c r="E58" t="n">
-        <v>24</v>
+        <v>3.6</v>
       </c>
       <c r="F58" t="n">
-        <v>10.45200438418203</v>
+        <v>-1.77635683940025e-15</v>
       </c>
       <c r="G58" t="n">
-        <v>6</v>
+        <v>71</v>
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>0x6</t>
+          <t>0x47</t>
         </is>
       </c>
       <c r="I58" t="n">
-        <v>11</v>
+        <v>72</v>
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>0xb</t>
+          <t>0x48</t>
         </is>
       </c>
     </row>
@@ -2832,34 +2832,34 @@
         <v>58</v>
       </c>
       <c r="B59" t="n">
-        <v>976.5668723469187</v>
+        <v>13.505</v>
       </c>
       <c r="C59" t="n">
-        <v>988</v>
+        <v>13.505</v>
       </c>
       <c r="D59" t="n">
-        <v>38</v>
+        <v>3.7</v>
       </c>
       <c r="E59" t="n">
-        <v>26</v>
+        <v>3.65</v>
       </c>
       <c r="F59" t="n">
-        <v>-11.43312765308133</v>
+        <v>-1.77635683940025e-15</v>
       </c>
       <c r="G59" t="n">
-        <v>6</v>
+        <v>70</v>
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>0x6</t>
+          <t>0x46</t>
         </is>
       </c>
       <c r="I59" t="n">
-        <v>9</v>
+        <v>71</v>
       </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t>0x9</t>
+          <t>0x47</t>
         </is>
       </c>
     </row>
@@ -2868,34 +2868,34 @@
         <v>59</v>
       </c>
       <c r="B60" t="n">
-        <v>1033.575438048704</v>
+        <v>13.6875</v>
       </c>
       <c r="C60" t="n">
-        <v>1034</v>
+        <v>13.6875</v>
       </c>
       <c r="D60" t="n">
-        <v>47</v>
+        <v>3.75</v>
       </c>
       <c r="E60" t="n">
-        <v>22</v>
+        <v>3.65</v>
       </c>
       <c r="F60" t="n">
-        <v>-0.4245619512955727</v>
+        <v>-1.77635683940025e-15</v>
       </c>
       <c r="G60" t="n">
-        <v>5</v>
+        <v>69</v>
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>0x5</t>
+          <t>0x45</t>
         </is>
       </c>
       <c r="I60" t="n">
-        <v>12</v>
+        <v>71</v>
       </c>
       <c r="J60" t="inlineStr">
         <is>
-          <t>0xc</t>
+          <t>0x47</t>
         </is>
       </c>
     </row>
@@ -2904,34 +2904,34 @@
         <v>60</v>
       </c>
       <c r="B61" t="n">
-        <v>1093.624303560184</v>
+        <v>14.0625</v>
       </c>
       <c r="C61" t="n">
-        <v>1120</v>
+        <v>14.0625</v>
       </c>
       <c r="D61" t="n">
-        <v>56</v>
+        <v>3.75</v>
       </c>
       <c r="E61" t="n">
-        <v>20</v>
+        <v>3.75</v>
       </c>
       <c r="F61" t="n">
-        <v>-26.37569643981601</v>
+        <v>-1.77635683940025e-15</v>
       </c>
       <c r="G61" t="n">
-        <v>4</v>
+        <v>69</v>
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>0x4</t>
+          <t>0x45</t>
         </is>
       </c>
       <c r="I61" t="n">
-        <v>13</v>
+        <v>69</v>
       </c>
       <c r="J61" t="inlineStr">
         <is>
-          <t>0xd</t>
+          <t>0x45</t>
         </is>
       </c>
     </row>
@@ -2940,34 +2940,34 @@
         <v>61</v>
       </c>
       <c r="B62" t="n">
-        <v>1156.867239831189</v>
+        <v>14.25</v>
       </c>
       <c r="C62" t="n">
-        <v>1175</v>
+        <v>14.25</v>
       </c>
       <c r="D62" t="n">
-        <v>47</v>
+        <v>3.8</v>
       </c>
       <c r="E62" t="n">
-        <v>25</v>
+        <v>3.75</v>
       </c>
       <c r="F62" t="n">
-        <v>-18.13276016881105</v>
+        <v>0</v>
       </c>
       <c r="G62" t="n">
-        <v>5</v>
+        <v>68</v>
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>0x5</t>
+          <t>0x44</t>
         </is>
       </c>
       <c r="I62" t="n">
-        <v>10</v>
+        <v>69</v>
       </c>
       <c r="J62" t="inlineStr">
         <is>
-          <t>0xa</t>
+          <t>0x45</t>
         </is>
       </c>
     </row>
@@ -2976,34 +2976,34 @@
         <v>62</v>
       </c>
       <c r="B63" t="n">
-        <v>1223.46552858894</v>
+        <v>14.63</v>
       </c>
       <c r="C63" t="n">
-        <v>1222</v>
+        <v>14.63</v>
       </c>
       <c r="D63" t="n">
-        <v>47</v>
+        <v>3.85</v>
       </c>
       <c r="E63" t="n">
-        <v>26</v>
+        <v>3.8</v>
       </c>
       <c r="F63" t="n">
-        <v>1.465528588939605</v>
+        <v>0</v>
       </c>
       <c r="G63" t="n">
-        <v>5</v>
+        <v>67</v>
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>0x5</t>
+          <t>0x43</t>
         </is>
       </c>
       <c r="I63" t="n">
-        <v>9</v>
+        <v>68</v>
       </c>
       <c r="J63" t="inlineStr">
         <is>
-          <t>0x9</t>
+          <t>0x44</t>
         </is>
       </c>
     </row>
@@ -3012,34 +3012,34 @@
         <v>63</v>
       </c>
       <c r="B64" t="n">
-        <v>1293.588320241202</v>
+        <v>15.015</v>
       </c>
       <c r="C64" t="n">
-        <v>1316</v>
+        <v>15.015</v>
       </c>
       <c r="D64" t="n">
-        <v>47</v>
+        <v>3.9</v>
       </c>
       <c r="E64" t="n">
-        <v>28</v>
+        <v>3.85</v>
       </c>
       <c r="F64" t="n">
-        <v>-22.4116797587983</v>
+        <v>-1.77635683940025e-15</v>
       </c>
       <c r="G64" t="n">
-        <v>5</v>
+        <v>66</v>
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>0x5</t>
+          <t>0x42</t>
         </is>
       </c>
       <c r="I64" t="n">
-        <v>8</v>
+        <v>67</v>
       </c>
       <c r="J64" t="inlineStr">
         <is>
-          <t>0x8</t>
+          <t>0x43</t>
         </is>
       </c>
     </row>
@@ -3048,34 +3048,34 @@
         <v>64</v>
       </c>
       <c r="B65" t="n">
-        <v>1367.413008522884</v>
+        <v>15.405</v>
       </c>
       <c r="C65" t="n">
-        <v>1380</v>
+        <v>15.405</v>
       </c>
       <c r="D65" t="n">
-        <v>69</v>
+        <v>3.95</v>
       </c>
       <c r="E65" t="n">
-        <v>20</v>
+        <v>3.9</v>
       </c>
       <c r="F65" t="n">
-        <v>-12.58699147711604</v>
+        <v>-1.77635683940025e-15</v>
       </c>
       <c r="G65" t="n">
-        <v>3</v>
+        <v>65</v>
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>0x3</t>
+          <t>0x41</t>
         </is>
       </c>
       <c r="I65" t="n">
-        <v>13</v>
+        <v>66</v>
       </c>
       <c r="J65" t="inlineStr">
         <is>
-          <t>0xd</t>
+          <t>0x42</t>
         </is>
       </c>
     </row>
@@ -3084,34 +3084,34 @@
         <v>65</v>
       </c>
       <c r="B66" t="n">
-        <v>1445.125622658268</v>
+        <v>15.6025</v>
       </c>
       <c r="C66" t="n">
-        <v>1444</v>
+        <v>15.6025</v>
       </c>
       <c r="D66" t="n">
-        <v>38</v>
+        <v>3.95</v>
       </c>
       <c r="E66" t="n">
-        <v>38</v>
+        <v>3.95</v>
       </c>
       <c r="F66" t="n">
-        <v>1.125622658267957</v>
+        <v>-1.77635683940025e-15</v>
       </c>
       <c r="G66" t="n">
-        <v>6</v>
+        <v>65</v>
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>0x6</t>
+          <t>0x41</t>
         </is>
       </c>
       <c r="I66" t="n">
-        <v>6</v>
+        <v>65</v>
       </c>
       <c r="J66" t="inlineStr">
         <is>
-          <t>0x6</t>
+          <t>0x41</t>
         </is>
       </c>
     </row>
@@ -3120,34 +3120,34 @@
         <v>66</v>
       </c>
       <c r="B67" t="n">
-        <v>1526.92123784631</v>
+        <v>15.7609</v>
       </c>
       <c r="C67" t="n">
-        <v>1518</v>
+        <v>15.7609</v>
       </c>
       <c r="D67" t="n">
-        <v>69</v>
+        <v>3.97</v>
       </c>
       <c r="E67" t="n">
-        <v>22</v>
+        <v>3.97</v>
       </c>
       <c r="F67" t="n">
-        <v>8.921237846309623</v>
+        <v>-3.552713678800501e-15</v>
       </c>
       <c r="G67" t="n">
-        <v>3</v>
+        <v>64</v>
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>0x3</t>
+          <t>0x40</t>
         </is>
       </c>
       <c r="I67" t="n">
-        <v>12</v>
+        <v>64</v>
       </c>
       <c r="J67" t="inlineStr">
         <is>
-          <t>0xc</t>
+          <t>0x40</t>
         </is>
       </c>
     </row>
@@ -3156,34 +3156,34 @@
         <v>67</v>
       </c>
       <c r="B68" t="n">
-        <v>1613.004404913173</v>
+        <v>15.88</v>
       </c>
       <c r="C68" t="n">
-        <v>1656</v>
+        <v>15.88</v>
       </c>
       <c r="D68" t="n">
-        <v>69</v>
+        <v>4</v>
       </c>
       <c r="E68" t="n">
-        <v>24</v>
+        <v>3.97</v>
       </c>
       <c r="F68" t="n">
-        <v>-42.99559508682682</v>
+        <v>0</v>
       </c>
       <c r="G68" t="n">
-        <v>3</v>
+        <v>63</v>
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>0x3</t>
+          <t>0x3f</t>
         </is>
       </c>
       <c r="I68" t="n">
-        <v>11</v>
+        <v>64</v>
       </c>
       <c r="J68" t="inlineStr">
         <is>
-          <t>0xb</t>
+          <t>0x40</t>
         </is>
       </c>
     </row>
@@ -3192,34 +3192,34 @@
         <v>68</v>
       </c>
       <c r="B69" t="n">
-        <v>1703.589600014695</v>
+        <v>16.4</v>
       </c>
       <c r="C69" t="n">
-        <v>1725</v>
+        <v>16.4</v>
       </c>
       <c r="D69" t="n">
-        <v>69</v>
+        <v>4.1</v>
       </c>
       <c r="E69" t="n">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="F69" t="n">
-        <v>-21.41039998530528</v>
+        <v>0</v>
       </c>
       <c r="G69" t="n">
-        <v>3</v>
+        <v>62</v>
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>0x3</t>
+          <t>0x3e</t>
         </is>
       </c>
       <c r="I69" t="n">
-        <v>10</v>
+        <v>63</v>
       </c>
       <c r="J69" t="inlineStr">
         <is>
-          <t>0xa</t>
+          <t>0x3f</t>
         </is>
       </c>
     </row>
@@ -3228,34 +3228,34 @@
         <v>69</v>
       </c>
       <c r="B70" t="n">
-        <v>1798.901695311646</v>
+        <v>16.81</v>
       </c>
       <c r="C70" t="n">
-        <v>1794</v>
+        <v>16.81</v>
       </c>
       <c r="D70" t="n">
-        <v>69</v>
+        <v>4.1</v>
       </c>
       <c r="E70" t="n">
-        <v>26</v>
+        <v>4.1</v>
       </c>
       <c r="F70" t="n">
-        <v>4.901695311645653</v>
+        <v>0</v>
       </c>
       <c r="G70" t="n">
-        <v>3</v>
+        <v>62</v>
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>0x3</t>
+          <t>0x3e</t>
         </is>
       </c>
       <c r="I70" t="n">
-        <v>9</v>
+        <v>62</v>
       </c>
       <c r="J70" t="inlineStr">
         <is>
-          <t>0x9</t>
+          <t>0x3e</t>
         </is>
       </c>
     </row>
@@ -3264,34 +3264,34 @@
         <v>70</v>
       </c>
       <c r="B71" t="n">
-        <v>1899.176451582651</v>
+        <v>17.64</v>
       </c>
       <c r="C71" t="n">
-        <v>1896</v>
+        <v>17.64</v>
       </c>
       <c r="D71" t="n">
-        <v>79</v>
+        <v>4.2</v>
       </c>
       <c r="E71" t="n">
-        <v>24</v>
+        <v>4.2</v>
       </c>
       <c r="F71" t="n">
-        <v>3.176451582650543</v>
+        <v>0</v>
       </c>
       <c r="G71" t="n">
-        <v>2</v>
+        <v>61</v>
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>0x2</t>
+          <t>0x3d</t>
         </is>
       </c>
       <c r="I71" t="n">
-        <v>11</v>
+        <v>61</v>
       </c>
       <c r="J71" t="inlineStr">
         <is>
-          <t>0xb</t>
+          <t>0x3d</t>
         </is>
       </c>
     </row>
@@ -3300,34 +3300,34 @@
         <v>71</v>
       </c>
       <c r="B72" t="n">
-        <v>2004.661033783607</v>
+        <v>18.06</v>
       </c>
       <c r="C72" t="n">
-        <v>1975</v>
+        <v>18.06</v>
       </c>
       <c r="D72" t="n">
-        <v>79</v>
+        <v>4.3</v>
       </c>
       <c r="E72" t="n">
-        <v>25</v>
+        <v>4.2</v>
       </c>
       <c r="F72" t="n">
-        <v>29.66103378360663</v>
+        <v>-3.552713678800501e-15</v>
       </c>
       <c r="G72" t="n">
-        <v>2</v>
+        <v>60</v>
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>0x2</t>
+          <t>0x3c</t>
         </is>
       </c>
       <c r="I72" t="n">
-        <v>10</v>
+        <v>61</v>
       </c>
       <c r="J72" t="inlineStr">
         <is>
-          <t>0xa</t>
+          <t>0x3d</t>
         </is>
       </c>
     </row>
@@ -3336,39 +3336,507 @@
         <v>72</v>
       </c>
       <c r="B73" t="n">
-        <v>2115.614550608168</v>
+        <v>18.48999999999999</v>
       </c>
       <c r="C73" t="n">
-        <v>2128</v>
+        <v>18.49</v>
       </c>
       <c r="D73" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="E73" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="F73" t="n">
+        <v>-3.552713678800501e-15</v>
+      </c>
+      <c r="G73" t="n">
+        <v>60</v>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>0x3c</t>
+        </is>
+      </c>
+      <c r="I73" t="n">
+        <v>60</v>
+      </c>
+      <c r="J73" t="inlineStr">
+        <is>
+          <t>0x3c</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>73</v>
+      </c>
+      <c r="B74" t="n">
+        <v>18.92</v>
+      </c>
+      <c r="C74" t="n">
+        <v>18.92</v>
+      </c>
+      <c r="D74" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="E74" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="F74" t="n">
+        <v>0</v>
+      </c>
+      <c r="G74" t="n">
+        <v>59</v>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>0x3b</t>
+        </is>
+      </c>
+      <c r="I74" t="n">
+        <v>60</v>
+      </c>
+      <c r="J74" t="inlineStr">
+        <is>
+          <t>0x3c</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>74</v>
+      </c>
+      <c r="B75" t="n">
+        <v>19.36</v>
+      </c>
+      <c r="C75" t="n">
+        <v>19.36</v>
+      </c>
+      <c r="D75" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="E75" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="F75" t="n">
+        <v>0</v>
+      </c>
+      <c r="G75" t="n">
+        <v>59</v>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>0x3b</t>
+        </is>
+      </c>
+      <c r="I75" t="n">
+        <v>59</v>
+      </c>
+      <c r="J75" t="inlineStr">
+        <is>
+          <t>0x3b</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>75</v>
+      </c>
+      <c r="B76" t="n">
+        <v>19.36</v>
+      </c>
+      <c r="C76" t="n">
+        <v>19.36</v>
+      </c>
+      <c r="D76" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="E76" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="F76" t="n">
+        <v>0</v>
+      </c>
+      <c r="G76" t="n">
+        <v>59</v>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>0x3b</t>
+        </is>
+      </c>
+      <c r="I76" t="n">
+        <v>59</v>
+      </c>
+      <c r="J76" t="inlineStr">
+        <is>
+          <t>0x3b</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>76</v>
+      </c>
+      <c r="B77" t="n">
+        <v>19.8</v>
+      </c>
+      <c r="C77" t="n">
+        <v>19.8</v>
+      </c>
+      <c r="D77" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E77" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="F77" t="n">
+        <v>0</v>
+      </c>
+      <c r="G77" t="n">
+        <v>58</v>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>0x3a</t>
+        </is>
+      </c>
+      <c r="I77" t="n">
+        <v>59</v>
+      </c>
+      <c r="J77" t="inlineStr">
+        <is>
+          <t>0x3b</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>77</v>
+      </c>
+      <c r="B78" t="n">
+        <v>20.25</v>
+      </c>
+      <c r="C78" t="n">
+        <v>20.25</v>
+      </c>
+      <c r="D78" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E78" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="F78" t="n">
+        <v>0</v>
+      </c>
+      <c r="G78" t="n">
+        <v>58</v>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>0x3a</t>
+        </is>
+      </c>
+      <c r="I78" t="n">
+        <v>58</v>
+      </c>
+      <c r="J78" t="inlineStr">
+        <is>
+          <t>0x3a</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>78</v>
+      </c>
+      <c r="B79" t="n">
+        <v>20.7</v>
+      </c>
+      <c r="C79" t="n">
+        <v>20.7</v>
+      </c>
+      <c r="D79" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="E79" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="F79" t="n">
+        <v>-3.552713678800501e-15</v>
+      </c>
+      <c r="G79" t="n">
+        <v>57</v>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>0x39</t>
+        </is>
+      </c>
+      <c r="I79" t="n">
+        <v>58</v>
+      </c>
+      <c r="J79" t="inlineStr">
+        <is>
+          <t>0x3a</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>79</v>
+      </c>
+      <c r="B80" t="n">
+        <v>21.15999999999999</v>
+      </c>
+      <c r="C80" t="n">
+        <v>21.16</v>
+      </c>
+      <c r="D80" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="E80" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="F80" t="n">
+        <v>-3.552713678800501e-15</v>
+      </c>
+      <c r="G80" t="n">
+        <v>57</v>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>0x39</t>
+        </is>
+      </c>
+      <c r="I80" t="n">
+        <v>57</v>
+      </c>
+      <c r="J80" t="inlineStr">
+        <is>
+          <t>0x39</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>80</v>
+      </c>
+      <c r="B81" t="n">
+        <v>21.15999999999999</v>
+      </c>
+      <c r="C81" t="n">
+        <v>21.16</v>
+      </c>
+      <c r="D81" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="E81" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="F81" t="n">
+        <v>-3.552713678800501e-15</v>
+      </c>
+      <c r="G81" t="n">
+        <v>57</v>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>0x39</t>
+        </is>
+      </c>
+      <c r="I81" t="n">
+        <v>57</v>
+      </c>
+      <c r="J81" t="inlineStr">
+        <is>
+          <t>0x39</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>81</v>
+      </c>
+      <c r="B82" t="n">
+        <v>21.62</v>
+      </c>
+      <c r="C82" t="n">
+        <v>21.62</v>
+      </c>
+      <c r="D82" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="E82" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="F82" t="n">
+        <v>0</v>
+      </c>
+      <c r="G82" t="n">
         <v>56</v>
       </c>
-      <c r="E73" t="n">
-        <v>38</v>
-      </c>
-      <c r="F73" t="n">
-        <v>-12.38544939183248</v>
-      </c>
-      <c r="G73" t="n">
-        <v>4</v>
-      </c>
-      <c r="H73" t="inlineStr">
-        <is>
-          <t>0x4</t>
-        </is>
-      </c>
-      <c r="I73" t="n">
-        <v>6</v>
-      </c>
-      <c r="J73" t="inlineStr">
-        <is>
-          <t>0x6</t>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>0x38</t>
+        </is>
+      </c>
+      <c r="I82" t="n">
+        <v>57</v>
+      </c>
+      <c r="J82" t="inlineStr">
+        <is>
+          <t>0x39</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>82</v>
+      </c>
+      <c r="B83" t="n">
+        <v>22.09</v>
+      </c>
+      <c r="C83" t="n">
+        <v>22.09</v>
+      </c>
+      <c r="D83" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="E83" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="F83" t="n">
+        <v>-3.552713678800501e-15</v>
+      </c>
+      <c r="G83" t="n">
+        <v>56</v>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>0x38</t>
+        </is>
+      </c>
+      <c r="I83" t="n">
+        <v>56</v>
+      </c>
+      <c r="J83" t="inlineStr">
+        <is>
+          <t>0x38</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>83</v>
+      </c>
+      <c r="B84" t="n">
+        <v>22.56</v>
+      </c>
+      <c r="C84" t="n">
+        <v>22.56</v>
+      </c>
+      <c r="D84" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="E84" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="F84" t="n">
+        <v>0</v>
+      </c>
+      <c r="G84" t="n">
+        <v>55</v>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>0x37</t>
+        </is>
+      </c>
+      <c r="I84" t="n">
+        <v>56</v>
+      </c>
+      <c r="J84" t="inlineStr">
+        <is>
+          <t>0x38</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>84</v>
+      </c>
+      <c r="B85" t="n">
+        <v>22.56</v>
+      </c>
+      <c r="C85" t="n">
+        <v>22.56</v>
+      </c>
+      <c r="D85" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="E85" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="F85" t="n">
+        <v>0</v>
+      </c>
+      <c r="G85" t="n">
+        <v>55</v>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>0x37</t>
+        </is>
+      </c>
+      <c r="I85" t="n">
+        <v>56</v>
+      </c>
+      <c r="J85" t="inlineStr">
+        <is>
+          <t>0x38</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>85</v>
+      </c>
+      <c r="B86" t="n">
+        <v>23.04</v>
+      </c>
+      <c r="C86" t="n">
+        <v>23.04</v>
+      </c>
+      <c r="D86" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="E86" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="F86" t="n">
+        <v>-3.552713678800501e-15</v>
+      </c>
+      <c r="G86" t="n">
+        <v>55</v>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>0x37</t>
+        </is>
+      </c>
+      <c r="I86" t="n">
+        <v>55</v>
+      </c>
+      <c r="J86" t="inlineStr">
+        <is>
+          <t>0x37</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>